<commit_message>
[lbmpi-3]: Updates & specgroup
</commit_message>
<xml_diff>
--- a/SupplementaryData.xlsx
+++ b/SupplementaryData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhsb1\Desktop\Results\LBE_DSLIM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhsb1\Documents\GitHub\lbdslim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94C15F2-B055-4E96-8C63-FBB0147B1E73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8607D312-2620-48A5-92DD-A7A6629C45FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11778" activeTab="2" xr2:uid="{0A13F19E-9CAF-425F-8126-E9E8F01A7964}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="76">
   <si>
     <t>Speedup</t>
   </si>
@@ -70,18 +70,9 @@
     <t>Experiment ran on 1 node only since 1 core</t>
   </si>
   <si>
-    <t>System Configurations Used</t>
-  </si>
-  <si>
     <t>No significant difference in results for either configuration</t>
   </si>
   <si>
-    <t>8 cores x 2 nodes</t>
-  </si>
-  <si>
-    <t>4 cores x 4 nodes</t>
-  </si>
-  <si>
     <t>Experiment Settings</t>
   </si>
   <si>
@@ -263,6 +254,12 @@
   </si>
   <si>
     <t>Please Note: At least 2 nodes in all experiments except green</t>
+  </si>
+  <si>
+    <t>UNCALIBRATED</t>
+  </si>
+  <si>
+    <t>CALIBRATED</t>
   </si>
 </sst>
 </file>
@@ -445,7 +442,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -477,6 +474,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -486,7 +492,7 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -510,6 +516,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="2" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -843,33 +853,33 @@
   <sheetData>
     <row r="2" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F7" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -877,52 +887,52 @@
     </row>
     <row r="10" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F17" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G19">
         <v>3</v>
@@ -930,15 +940,15 @@
     </row>
     <row r="20" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F21" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G21">
         <v>100</v>
@@ -946,7 +956,7 @@
     </row>
     <row r="22" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G22">
         <v>39</v>
@@ -954,23 +964,23 @@
     </row>
     <row r="23" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F23" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F24" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F25" s="16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G25">
         <v>4</v>
@@ -978,79 +988,79 @@
     </row>
     <row r="26" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F26" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F27" s="16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F28" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G28" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F29" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F32" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F34" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G34" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F35" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G35" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F36" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G36" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F37" t="s">
+        <v>49</v>
+      </c>
+      <c r="G37" t="s">
         <v>52</v>
-      </c>
-      <c r="G37" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="38" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F38" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G38" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1080,45 +1090,45 @@
   <sheetData>
     <row r="1" spans="3:12" ht="28.5" thickBot="1" x14ac:dyDescent="1.1000000000000001">
       <c r="F1" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="3:12" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="4" spans="3:12" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="3:12" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>66</v>
-      </c>
       <c r="I6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="L6" s="19" t="s">
         <v>63</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="L6" s="19" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.55000000000000004">
@@ -1271,7 +1281,7 @@
         <v>7</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J13" s="21">
         <f>AVERAGE(J7:J11)</f>
@@ -1288,7 +1298,7 @@
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.55000000000000004">
       <c r="I14" s="21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J14" s="21">
         <f>J13*100</f>
@@ -1305,16 +1315,16 @@
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="19" t="s">
         <v>63</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.55000000000000004">
@@ -1359,7 +1369,7 @@
         <v>116.95</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.55000000000000004">
@@ -1390,16 +1400,16 @@
         <v>141.05000000000001</v>
       </c>
       <c r="I20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="L20" s="19" t="s">
         <v>63</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="K20" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="L20" s="19" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.55000000000000004">
@@ -1421,7 +1431,7 @@
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.55000000000000004">
       <c r="C22" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I22">
         <v>18</v>
@@ -1458,16 +1468,16 @@
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="19" t="s">
         <v>63</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>66</v>
       </c>
       <c r="I24">
         <v>41</v>
@@ -1551,7 +1561,7 @@
         <v>21.25</v>
       </c>
       <c r="I27" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J27" s="21">
         <f>AVERAGE(J21:J25)</f>
@@ -1583,7 +1593,7 @@
         <v>36.900000000000006</v>
       </c>
       <c r="I28" s="21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J28" s="21">
         <f>J27*100</f>
@@ -1623,10 +1633,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D67BCB2-126E-41B0-B29E-49CCB1AA2A48}">
-  <dimension ref="A1:W36"/>
+  <dimension ref="A1:W56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1640,7 +1650,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="28.5" thickBot="1" x14ac:dyDescent="1.1000000000000001">
       <c r="H1" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="O1" s="10"/>
       <c r="P1" s="10"/>
@@ -1649,7 +1659,7 @@
     <row r="2" spans="1:23" ht="20.7" thickTop="1" x14ac:dyDescent="0.75">
       <c r="A2" s="2"/>
       <c r="M2" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
@@ -1672,13 +1682,9 @@
       <c r="M4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="14" t="s">
-        <v>15</v>
-      </c>
+      <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
-      <c r="R4" s="14" t="s">
-        <v>14</v>
-      </c>
+      <c r="R4" s="14"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2"/>
@@ -1694,7 +1700,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="7"/>
       <c r="M5" s="2" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.55000000000000004">
@@ -1707,9 +1713,6 @@
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="4"/>
-      <c r="M6" s="2" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="11"/>
@@ -2085,7 +2088,9 @@
       <c r="C19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J19" s="2"/>
+      <c r="J19" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="K19" s="1" t="s">
         <v>1</v>
       </c>
@@ -2500,6 +2505,9 @@
       <c r="C29" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="J29" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="K29" s="1" t="s">
         <v>3</v>
       </c>
@@ -2549,7 +2557,9 @@
       <c r="O31" s="2">
         <v>16</v>
       </c>
-      <c r="P31" s="2"/>
+      <c r="P31" s="23" t="s">
+        <v>64</v>
+      </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="2" t="s">
         <v>4</v>
@@ -2615,6 +2625,10 @@
         <f t="shared" si="16"/>
         <v>1.0898267326732671</v>
       </c>
+      <c r="P32">
+        <f>AVERAGE(L32:O32)</f>
+        <v>1.0275145035915501</v>
+      </c>
       <c r="R32" s="2">
         <v>4</v>
       </c>
@@ -2683,6 +2697,10 @@
         <f t="shared" si="19"/>
         <v>1.0357245071019716</v>
       </c>
+      <c r="P33">
+        <f>AVERAGE(M33:O33)</f>
+        <v>0.98142913977256285</v>
+      </c>
       <c r="R33" s="2">
         <v>18</v>
       </c>
@@ -2749,6 +2767,10 @@
         <f t="shared" si="22"/>
         <v>0.95533053774050325</v>
       </c>
+      <c r="P34">
+        <f>AVERAGE(N34:O34)</f>
+        <v>0.92736778252536256</v>
+      </c>
       <c r="R34" s="2">
         <v>30</v>
       </c>
@@ -2814,6 +2836,10 @@
         <f t="shared" si="25"/>
         <v>0.91404033764616333</v>
       </c>
+      <c r="P35">
+        <f t="shared" ref="P35:P36" si="26">AVERAGE(N35:O35)</f>
+        <v>0.9289461860416719</v>
+      </c>
       <c r="R35" s="2">
         <v>41</v>
       </c>
@@ -2828,11 +2854,11 @@
         <v>1</v>
       </c>
       <c r="V35">
-        <f t="shared" ref="V35:W35" si="26">V25/V31</f>
+        <f t="shared" ref="V35:W35" si="27">V25/V31</f>
         <v>0.83757812387234609</v>
       </c>
       <c r="W35">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.66098678290320512</v>
       </c>
     </row>
@@ -2851,11 +2877,11 @@
         <v>1</v>
       </c>
       <c r="F36">
-        <f t="shared" ref="F36:G36" si="27">F26/F31</f>
+        <f t="shared" ref="F36:G36" si="28">F26/F31</f>
         <v>1.0264672260732093</v>
       </c>
       <c r="G36">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.95750975587621379</v>
       </c>
       <c r="J36" s="2">
@@ -2872,12 +2898,16 @@
         <v>1</v>
       </c>
       <c r="N36">
-        <f t="shared" ref="N36:O36" si="28">N26/N31</f>
+        <f t="shared" ref="N36:O36" si="29">N26/N31</f>
         <v>1.0309484573835026</v>
       </c>
       <c r="O36">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.92538828169940013</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="26"/>
+        <v>0.97816836954145137</v>
       </c>
       <c r="R36" s="2">
         <v>49</v>
@@ -2893,12 +2923,300 @@
         <v>1</v>
       </c>
       <c r="V36">
-        <f t="shared" ref="V36:W36" si="29">V26/V31</f>
+        <f t="shared" ref="V36:W36" si="30">V26/V31</f>
         <v>0.86865059297797509</v>
       </c>
       <c r="W36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.60310120882477791</v>
+      </c>
+    </row>
+    <row r="39" spans="2:23" ht="17.100000000000001" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="J39" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:23" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="J41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K41" s="2">
+        <v>1</v>
+      </c>
+      <c r="L41" s="2">
+        <v>2</v>
+      </c>
+      <c r="M41" s="2">
+        <v>4</v>
+      </c>
+      <c r="N41" s="2">
+        <v>8</v>
+      </c>
+      <c r="O41" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="J42" s="2">
+        <v>4</v>
+      </c>
+      <c r="K42" s="12">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>1.8528904288299406</v>
+      </c>
+      <c r="M42">
+        <v>4.104630205096333</v>
+      </c>
+      <c r="N42">
+        <v>8.5410281280310372</v>
+      </c>
+      <c r="O42">
+        <v>17.437227722772274</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="J43" s="2">
+        <v>18</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L43" s="4">
+        <f>L23*0.9814</f>
+        <v>1.9628000000000001</v>
+      </c>
+      <c r="M43" s="4">
+        <f t="shared" ref="M43:O43" si="31">M23*0.9814</f>
+        <v>3.7783208798353018</v>
+      </c>
+      <c r="N43" s="4">
+        <f t="shared" si="31"/>
+        <v>7.4278673767174359</v>
+      </c>
+      <c r="O43" s="4">
+        <f t="shared" si="31"/>
+        <v>16.263360500318001</v>
+      </c>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="J44" s="2">
+        <v>30</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L44" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M44" s="4">
+        <f>M24*0.9273</f>
+        <v>3.7092000000000001</v>
+      </c>
+      <c r="N44" s="4">
+        <f t="shared" ref="N44:O44" si="32">N24*0.9273</f>
+        <v>6.6721462545981494</v>
+      </c>
+      <c r="O44" s="4">
+        <f t="shared" si="32"/>
+        <v>14.174048122348299</v>
+      </c>
+    </row>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="J45" s="2">
+        <v>41</v>
+      </c>
+      <c r="K45" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M45" s="4">
+        <f>M25*0.9289</f>
+        <v>3.7155999999999998</v>
+      </c>
+      <c r="N45" s="4">
+        <f t="shared" ref="N45:O45" si="33">N25*0.9289</f>
+        <v>7.0139532383095755</v>
+      </c>
+      <c r="O45" s="4">
+        <f t="shared" si="33"/>
+        <v>13.584833114232337</v>
+      </c>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="J46" s="2">
+        <v>49</v>
+      </c>
+      <c r="K46" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L46" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M46" s="4">
+        <f>M26*0.9781</f>
+        <v>3.9123999999999999</v>
+      </c>
+      <c r="N46" s="4">
+        <f t="shared" ref="N46:O46" si="34">N26*0.9781</f>
+        <v>8.0669654893344305</v>
+      </c>
+      <c r="O46" s="4">
+        <f t="shared" si="34"/>
+        <v>14.481956453282931</v>
+      </c>
+    </row>
+    <row r="49" spans="10:15" ht="17.100000000000001" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="J49" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="10:15" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="51" spans="10:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="J51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K51" s="2">
+        <v>1</v>
+      </c>
+      <c r="L51" s="2">
+        <v>2</v>
+      </c>
+      <c r="M51" s="2">
+        <v>4</v>
+      </c>
+      <c r="N51" s="2">
+        <v>8</v>
+      </c>
+      <c r="O51" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="10:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="J52" s="2">
+        <v>4</v>
+      </c>
+      <c r="K52" s="4">
+        <v>1</v>
+      </c>
+      <c r="L52">
+        <f>L42/L51</f>
+        <v>0.9264452144149703</v>
+      </c>
+      <c r="M52">
+        <f t="shared" ref="M52:O52" si="35">M42/M51</f>
+        <v>1.0261575512740833</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="35"/>
+        <v>1.0676285160038796</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="35"/>
+        <v>1.0898267326732671</v>
+      </c>
+    </row>
+    <row r="53" spans="10:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="J53" s="2">
+        <v>18</v>
+      </c>
+      <c r="K53" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L53" s="24">
+        <f>L43/L51</f>
+        <v>0.98140000000000005</v>
+      </c>
+      <c r="M53">
+        <f t="shared" ref="M53:O53" si="36">M43/M51</f>
+        <v>0.94458021995882546</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="36"/>
+        <v>0.92848342208967949</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="36"/>
+        <v>1.0164600312698751</v>
+      </c>
+    </row>
+    <row r="54" spans="10:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="J54" s="2">
+        <v>30</v>
+      </c>
+      <c r="K54" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L54" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M54" s="4">
+        <f>M44/M51</f>
+        <v>0.92730000000000001</v>
+      </c>
+      <c r="N54">
+        <f t="shared" ref="N54:O54" si="37">N44/N51</f>
+        <v>0.83401828182476867</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="37"/>
+        <v>0.88587800764676872</v>
+      </c>
+    </row>
+    <row r="55" spans="10:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="J55" s="2">
+        <v>41</v>
+      </c>
+      <c r="K55" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L55" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M55" s="4">
+        <f>M45/M51</f>
+        <v>0.92889999999999995</v>
+      </c>
+      <c r="N55">
+        <f t="shared" ref="N55:O55" si="38">N45/N51</f>
+        <v>0.87674415478869694</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="38"/>
+        <v>0.84905206963952107</v>
+      </c>
+    </row>
+    <row r="56" spans="10:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="J56" s="2">
+        <v>49</v>
+      </c>
+      <c r="K56" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L56" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M56" s="4">
+        <f>M46/M51</f>
+        <v>0.97809999999999997</v>
+      </c>
+      <c r="N56">
+        <f t="shared" ref="N56:O56" si="39">N46/N51</f>
+        <v>1.0083706861668038</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="39"/>
+        <v>0.90512227833018322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[lbircc-2]: Add specgroup and update SuppData
</commit_message>
<xml_diff>
--- a/SupplementaryData.xlsx
+++ b/SupplementaryData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhsb1\Desktop\Results\LBE_DSLIM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhsb1\Documents\GitHub\lbdslim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94C15F2-B055-4E96-8C63-FBB0147B1E73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8607D312-2620-48A5-92DD-A7A6629C45FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11778" activeTab="2" xr2:uid="{0A13F19E-9CAF-425F-8126-E9E8F01A7964}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="76">
   <si>
     <t>Speedup</t>
   </si>
@@ -70,18 +70,9 @@
     <t>Experiment ran on 1 node only since 1 core</t>
   </si>
   <si>
-    <t>System Configurations Used</t>
-  </si>
-  <si>
     <t>No significant difference in results for either configuration</t>
   </si>
   <si>
-    <t>8 cores x 2 nodes</t>
-  </si>
-  <si>
-    <t>4 cores x 4 nodes</t>
-  </si>
-  <si>
     <t>Experiment Settings</t>
   </si>
   <si>
@@ -263,6 +254,12 @@
   </si>
   <si>
     <t>Please Note: At least 2 nodes in all experiments except green</t>
+  </si>
+  <si>
+    <t>UNCALIBRATED</t>
+  </si>
+  <si>
+    <t>CALIBRATED</t>
   </si>
 </sst>
 </file>
@@ -445,7 +442,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -477,6 +474,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -486,7 +492,7 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -510,6 +516,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="2" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -843,33 +853,33 @@
   <sheetData>
     <row r="2" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F7" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -877,52 +887,52 @@
     </row>
     <row r="10" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F17" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G19">
         <v>3</v>
@@ -930,15 +940,15 @@
     </row>
     <row r="20" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F21" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G21">
         <v>100</v>
@@ -946,7 +956,7 @@
     </row>
     <row r="22" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G22">
         <v>39</v>
@@ -954,23 +964,23 @@
     </row>
     <row r="23" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F23" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F24" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F25" s="16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G25">
         <v>4</v>
@@ -978,79 +988,79 @@
     </row>
     <row r="26" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F26" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F27" s="16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F28" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G28" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F29" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F32" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F34" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G34" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F35" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G35" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F36" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G36" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F37" t="s">
+        <v>49</v>
+      </c>
+      <c r="G37" t="s">
         <v>52</v>
-      </c>
-      <c r="G37" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="38" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F38" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G38" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1080,45 +1090,45 @@
   <sheetData>
     <row r="1" spans="3:12" ht="28.5" thickBot="1" x14ac:dyDescent="1.1000000000000001">
       <c r="F1" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="3:12" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="4" spans="3:12" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="3:12" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>66</v>
-      </c>
       <c r="I6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="L6" s="19" t="s">
         <v>63</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="L6" s="19" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.55000000000000004">
@@ -1271,7 +1281,7 @@
         <v>7</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J13" s="21">
         <f>AVERAGE(J7:J11)</f>
@@ -1288,7 +1298,7 @@
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.55000000000000004">
       <c r="I14" s="21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J14" s="21">
         <f>J13*100</f>
@@ -1305,16 +1315,16 @@
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="19" t="s">
         <v>63</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.55000000000000004">
@@ -1359,7 +1369,7 @@
         <v>116.95</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.55000000000000004">
@@ -1390,16 +1400,16 @@
         <v>141.05000000000001</v>
       </c>
       <c r="I20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="L20" s="19" t="s">
         <v>63</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="K20" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="L20" s="19" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.55000000000000004">
@@ -1421,7 +1431,7 @@
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.55000000000000004">
       <c r="C22" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I22">
         <v>18</v>
@@ -1458,16 +1468,16 @@
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="19" t="s">
         <v>63</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>66</v>
       </c>
       <c r="I24">
         <v>41</v>
@@ -1551,7 +1561,7 @@
         <v>21.25</v>
       </c>
       <c r="I27" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J27" s="21">
         <f>AVERAGE(J21:J25)</f>
@@ -1583,7 +1593,7 @@
         <v>36.900000000000006</v>
       </c>
       <c r="I28" s="21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J28" s="21">
         <f>J27*100</f>
@@ -1623,10 +1633,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D67BCB2-126E-41B0-B29E-49CCB1AA2A48}">
-  <dimension ref="A1:W36"/>
+  <dimension ref="A1:W56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1640,7 +1650,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="28.5" thickBot="1" x14ac:dyDescent="1.1000000000000001">
       <c r="H1" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="O1" s="10"/>
       <c r="P1" s="10"/>
@@ -1649,7 +1659,7 @@
     <row r="2" spans="1:23" ht="20.7" thickTop="1" x14ac:dyDescent="0.75">
       <c r="A2" s="2"/>
       <c r="M2" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
@@ -1672,13 +1682,9 @@
       <c r="M4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="14" t="s">
-        <v>15</v>
-      </c>
+      <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
-      <c r="R4" s="14" t="s">
-        <v>14</v>
-      </c>
+      <c r="R4" s="14"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2"/>
@@ -1694,7 +1700,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="7"/>
       <c r="M5" s="2" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.55000000000000004">
@@ -1707,9 +1713,6 @@
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="4"/>
-      <c r="M6" s="2" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="11"/>
@@ -2085,7 +2088,9 @@
       <c r="C19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J19" s="2"/>
+      <c r="J19" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="K19" s="1" t="s">
         <v>1</v>
       </c>
@@ -2500,6 +2505,9 @@
       <c r="C29" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="J29" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="K29" s="1" t="s">
         <v>3</v>
       </c>
@@ -2549,7 +2557,9 @@
       <c r="O31" s="2">
         <v>16</v>
       </c>
-      <c r="P31" s="2"/>
+      <c r="P31" s="23" t="s">
+        <v>64</v>
+      </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="2" t="s">
         <v>4</v>
@@ -2615,6 +2625,10 @@
         <f t="shared" si="16"/>
         <v>1.0898267326732671</v>
       </c>
+      <c r="P32">
+        <f>AVERAGE(L32:O32)</f>
+        <v>1.0275145035915501</v>
+      </c>
       <c r="R32" s="2">
         <v>4</v>
       </c>
@@ -2683,6 +2697,10 @@
         <f t="shared" si="19"/>
         <v>1.0357245071019716</v>
       </c>
+      <c r="P33">
+        <f>AVERAGE(M33:O33)</f>
+        <v>0.98142913977256285</v>
+      </c>
       <c r="R33" s="2">
         <v>18</v>
       </c>
@@ -2749,6 +2767,10 @@
         <f t="shared" si="22"/>
         <v>0.95533053774050325</v>
       </c>
+      <c r="P34">
+        <f>AVERAGE(N34:O34)</f>
+        <v>0.92736778252536256</v>
+      </c>
       <c r="R34" s="2">
         <v>30</v>
       </c>
@@ -2814,6 +2836,10 @@
         <f t="shared" si="25"/>
         <v>0.91404033764616333</v>
       </c>
+      <c r="P35">
+        <f t="shared" ref="P35:P36" si="26">AVERAGE(N35:O35)</f>
+        <v>0.9289461860416719</v>
+      </c>
       <c r="R35" s="2">
         <v>41</v>
       </c>
@@ -2828,11 +2854,11 @@
         <v>1</v>
       </c>
       <c r="V35">
-        <f t="shared" ref="V35:W35" si="26">V25/V31</f>
+        <f t="shared" ref="V35:W35" si="27">V25/V31</f>
         <v>0.83757812387234609</v>
       </c>
       <c r="W35">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.66098678290320512</v>
       </c>
     </row>
@@ -2851,11 +2877,11 @@
         <v>1</v>
       </c>
       <c r="F36">
-        <f t="shared" ref="F36:G36" si="27">F26/F31</f>
+        <f t="shared" ref="F36:G36" si="28">F26/F31</f>
         <v>1.0264672260732093</v>
       </c>
       <c r="G36">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.95750975587621379</v>
       </c>
       <c r="J36" s="2">
@@ -2872,12 +2898,16 @@
         <v>1</v>
       </c>
       <c r="N36">
-        <f t="shared" ref="N36:O36" si="28">N26/N31</f>
+        <f t="shared" ref="N36:O36" si="29">N26/N31</f>
         <v>1.0309484573835026</v>
       </c>
       <c r="O36">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.92538828169940013</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="26"/>
+        <v>0.97816836954145137</v>
       </c>
       <c r="R36" s="2">
         <v>49</v>
@@ -2893,12 +2923,300 @@
         <v>1</v>
       </c>
       <c r="V36">
-        <f t="shared" ref="V36:W36" si="29">V26/V31</f>
+        <f t="shared" ref="V36:W36" si="30">V26/V31</f>
         <v>0.86865059297797509</v>
       </c>
       <c r="W36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.60310120882477791</v>
+      </c>
+    </row>
+    <row r="39" spans="2:23" ht="17.100000000000001" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="J39" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:23" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="J41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K41" s="2">
+        <v>1</v>
+      </c>
+      <c r="L41" s="2">
+        <v>2</v>
+      </c>
+      <c r="M41" s="2">
+        <v>4</v>
+      </c>
+      <c r="N41" s="2">
+        <v>8</v>
+      </c>
+      <c r="O41" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="J42" s="2">
+        <v>4</v>
+      </c>
+      <c r="K42" s="12">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>1.8528904288299406</v>
+      </c>
+      <c r="M42">
+        <v>4.104630205096333</v>
+      </c>
+      <c r="N42">
+        <v>8.5410281280310372</v>
+      </c>
+      <c r="O42">
+        <v>17.437227722772274</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="J43" s="2">
+        <v>18</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L43" s="4">
+        <f>L23*0.9814</f>
+        <v>1.9628000000000001</v>
+      </c>
+      <c r="M43" s="4">
+        <f t="shared" ref="M43:O43" si="31">M23*0.9814</f>
+        <v>3.7783208798353018</v>
+      </c>
+      <c r="N43" s="4">
+        <f t="shared" si="31"/>
+        <v>7.4278673767174359</v>
+      </c>
+      <c r="O43" s="4">
+        <f t="shared" si="31"/>
+        <v>16.263360500318001</v>
+      </c>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="J44" s="2">
+        <v>30</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L44" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M44" s="4">
+        <f>M24*0.9273</f>
+        <v>3.7092000000000001</v>
+      </c>
+      <c r="N44" s="4">
+        <f t="shared" ref="N44:O44" si="32">N24*0.9273</f>
+        <v>6.6721462545981494</v>
+      </c>
+      <c r="O44" s="4">
+        <f t="shared" si="32"/>
+        <v>14.174048122348299</v>
+      </c>
+    </row>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="J45" s="2">
+        <v>41</v>
+      </c>
+      <c r="K45" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M45" s="4">
+        <f>M25*0.9289</f>
+        <v>3.7155999999999998</v>
+      </c>
+      <c r="N45" s="4">
+        <f t="shared" ref="N45:O45" si="33">N25*0.9289</f>
+        <v>7.0139532383095755</v>
+      </c>
+      <c r="O45" s="4">
+        <f t="shared" si="33"/>
+        <v>13.584833114232337</v>
+      </c>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="J46" s="2">
+        <v>49</v>
+      </c>
+      <c r="K46" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L46" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M46" s="4">
+        <f>M26*0.9781</f>
+        <v>3.9123999999999999</v>
+      </c>
+      <c r="N46" s="4">
+        <f t="shared" ref="N46:O46" si="34">N26*0.9781</f>
+        <v>8.0669654893344305</v>
+      </c>
+      <c r="O46" s="4">
+        <f t="shared" si="34"/>
+        <v>14.481956453282931</v>
+      </c>
+    </row>
+    <row r="49" spans="10:15" ht="17.100000000000001" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="J49" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="10:15" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="51" spans="10:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="J51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K51" s="2">
+        <v>1</v>
+      </c>
+      <c r="L51" s="2">
+        <v>2</v>
+      </c>
+      <c r="M51" s="2">
+        <v>4</v>
+      </c>
+      <c r="N51" s="2">
+        <v>8</v>
+      </c>
+      <c r="O51" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="10:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="J52" s="2">
+        <v>4</v>
+      </c>
+      <c r="K52" s="4">
+        <v>1</v>
+      </c>
+      <c r="L52">
+        <f>L42/L51</f>
+        <v>0.9264452144149703</v>
+      </c>
+      <c r="M52">
+        <f t="shared" ref="M52:O52" si="35">M42/M51</f>
+        <v>1.0261575512740833</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="35"/>
+        <v>1.0676285160038796</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="35"/>
+        <v>1.0898267326732671</v>
+      </c>
+    </row>
+    <row r="53" spans="10:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="J53" s="2">
+        <v>18</v>
+      </c>
+      <c r="K53" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L53" s="24">
+        <f>L43/L51</f>
+        <v>0.98140000000000005</v>
+      </c>
+      <c r="M53">
+        <f t="shared" ref="M53:O53" si="36">M43/M51</f>
+        <v>0.94458021995882546</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="36"/>
+        <v>0.92848342208967949</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="36"/>
+        <v>1.0164600312698751</v>
+      </c>
+    </row>
+    <row r="54" spans="10:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="J54" s="2">
+        <v>30</v>
+      </c>
+      <c r="K54" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L54" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M54" s="4">
+        <f>M44/M51</f>
+        <v>0.92730000000000001</v>
+      </c>
+      <c r="N54">
+        <f t="shared" ref="N54:O54" si="37">N44/N51</f>
+        <v>0.83401828182476867</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="37"/>
+        <v>0.88587800764676872</v>
+      </c>
+    </row>
+    <row r="55" spans="10:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="J55" s="2">
+        <v>41</v>
+      </c>
+      <c r="K55" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L55" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M55" s="4">
+        <f>M45/M51</f>
+        <v>0.92889999999999995</v>
+      </c>
+      <c r="N55">
+        <f t="shared" ref="N55:O55" si="38">N45/N51</f>
+        <v>0.87674415478869694</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="38"/>
+        <v>0.84905206963952107</v>
+      </c>
+    </row>
+    <row r="56" spans="10:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="J56" s="2">
+        <v>49</v>
+      </c>
+      <c r="K56" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L56" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M56" s="4">
+        <f>M46/M51</f>
+        <v>0.97809999999999997</v>
+      </c>
+      <c r="N56">
+        <f t="shared" ref="N56:O56" si="39">N46/N51</f>
+        <v>1.0083706861668038</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="39"/>
+        <v>0.90512227833018322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>